<commit_message>
Dodano widok sklepu, drak mode, scheme od shoes
</commit_message>
<xml_diff>
--- a/newslatter.xlsx
+++ b/newslatter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>fdsfds@o2.pl</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>jifjlfdkfsd@02.pl</t>
+  </si>
+  <si>
+    <t>noeloo@o2.pl</t>
+  </si>
+  <si>
+    <t>michaltak830@gmail.com</t>
+  </si>
+  <si>
+    <t>takk@o2.pl</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D6" sqref="D6"/>
@@ -581,6 +590,21 @@
         <v>19</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>